<commit_message>
CKU overall advancement. Some minor code changes
</commit_message>
<xml_diff>
--- a/src/Input_Files/characters/francia_characters.xlsx
+++ b/src/Input_Files/characters/francia_characters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Desktop\CK\CKU_bestanden\Mapping\france_export_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07017816-128C-4EAA-AC1D-327BE094B71D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BEF35C-62FB-4F10-A955-062A734F1BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E5B2FA9E-FCEB-4F64-AA77-9CDFE63EBBF9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{E5B2FA9E-FCEB-4F64-AA77-9CDFE63EBBF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="410">
   <si>
     <t>RGB</t>
   </si>
@@ -264,12 +264,6 @@
     <t>(245, 10, 183)</t>
   </si>
   <si>
-    <t>CKU_artois_5</t>
-  </si>
-  <si>
-    <t>(186, 148, 69)</t>
-  </si>
-  <si>
     <t>CKU_anjou_13</t>
   </si>
   <si>
@@ -459,12 +453,6 @@
     <t>(40, 103, 75)</t>
   </si>
   <si>
-    <t>CKU_tour_auvergne_2</t>
-  </si>
-  <si>
-    <t>(118, 108, 108)</t>
-  </si>
-  <si>
     <t>CKU_alencon_7</t>
   </si>
   <si>
@@ -765,9 +753,6 @@
     <t>CKU_uzes_24</t>
   </si>
   <si>
-    <t>(36, 168, 249)</t>
-  </si>
-  <si>
     <t>CKU_francien_minor_45</t>
   </si>
   <si>
@@ -1138,6 +1123,147 @@
   </si>
   <si>
     <t>CKU_francien_minor_77</t>
+  </si>
+  <si>
+    <t>CKU_alsace_29</t>
+  </si>
+  <si>
+    <t>(129, 226, 12)</t>
+  </si>
+  <si>
+    <t>CKU_berghes_10</t>
+  </si>
+  <si>
+    <t>(166, 71, 59)</t>
+  </si>
+  <si>
+    <t>(195, 106, 22)</t>
+  </si>
+  <si>
+    <t>CKU_egmont_34</t>
+  </si>
+  <si>
+    <t>(76, 201, 23)</t>
+  </si>
+  <si>
+    <t>CKU_german_minor_9</t>
+  </si>
+  <si>
+    <t>(57, 164, 46)</t>
+  </si>
+  <si>
+    <t>CKU_nassau_44</t>
+  </si>
+  <si>
+    <t>CKU_zuylen_12</t>
+  </si>
+  <si>
+    <t>(150, 151, 60)</t>
+  </si>
+  <si>
+    <t>CKU_german_minor_10</t>
+  </si>
+  <si>
+    <t>(116, 215, 24)</t>
+  </si>
+  <si>
+    <t>CKU_bourgogne_minor_13</t>
+  </si>
+  <si>
+    <t>(62, 180, 24)</t>
+  </si>
+  <si>
+    <t>CKU_la_tour_2</t>
+  </si>
+  <si>
+    <t>(118, 108, 188)</t>
+  </si>
+  <si>
+    <t>e_hre</t>
+  </si>
+  <si>
+    <t>CKU_stewart_164</t>
+  </si>
+  <si>
+    <t>(251, 42, 234)</t>
+  </si>
+  <si>
+    <t>CKU_boppard_6</t>
+  </si>
+  <si>
+    <t>(225, 238, 235)</t>
+  </si>
+  <si>
+    <t>(80, 75, 7)</t>
+  </si>
+  <si>
+    <t>(121, 74, 86)</t>
+  </si>
+  <si>
+    <t>CKU_francien_minor_79</t>
+  </si>
+  <si>
+    <t>CKU_francien_minor_80</t>
+  </si>
+  <si>
+    <t>CKU_francien_minor_81</t>
+  </si>
+  <si>
+    <t>CKU_francien_minor_82</t>
+  </si>
+  <si>
+    <t>CKU_francien_minor_83</t>
+  </si>
+  <si>
+    <t>CKU_francien_minor_84</t>
+  </si>
+  <si>
+    <t>CKU_francien_minor_85</t>
+  </si>
+  <si>
+    <t>CKU_francien_minor_86</t>
+  </si>
+  <si>
+    <t>CKU_francien_minor_87</t>
+  </si>
+  <si>
+    <t>CKU_francien_minor_88</t>
+  </si>
+  <si>
+    <t>CKU_francien_minor_89</t>
+  </si>
+  <si>
+    <t>(32, 182, 133)</t>
+  </si>
+  <si>
+    <t>(69, 247, 9)</t>
+  </si>
+  <si>
+    <t>(195, 210, 182)</t>
+  </si>
+  <si>
+    <t>(239, 111, 83)</t>
+  </si>
+  <si>
+    <t>(93, 79, 16)</t>
+  </si>
+  <si>
+    <t>(121, 51, 125)</t>
+  </si>
+  <si>
+    <t>(75, 114, 228)</t>
+  </si>
+  <si>
+    <t>(55, 5, 211)</t>
+  </si>
+  <si>
+    <t>(59, 142, 58)</t>
+  </si>
+  <si>
+    <t>d_savoue</t>
+  </si>
+  <si>
+    <t>(15, 132, 243)</t>
   </si>
 </sst>
 </file>
@@ -1186,7 +1312,227 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1537,42 +1883,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{400C5842-DB98-492E-993D-80D39F62EB82}">
-  <dimension ref="A1:BD156"/>
+  <dimension ref="A1:BD174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="A154" sqref="A154"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L168" sqref="L168"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="5.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1742,7 +2088,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
@@ -1753,7 +2099,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
@@ -1767,7 +2113,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>61</v>
       </c>
@@ -1781,7 +2127,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>63</v>
       </c>
@@ -1795,7 +2141,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>65</v>
       </c>
@@ -1809,7 +2155,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -1819,9 +2165,11 @@
       <c r="D7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="H7" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="8" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -1835,7 +2183,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -1849,7 +2197,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -1863,7 +2211,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>76</v>
       </c>
@@ -1877,7 +2225,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>78</v>
       </c>
@@ -1891,7 +2239,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>80</v>
       </c>
@@ -1905,23 +2253,23 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>82</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>86</v>
@@ -1929,25 +2277,25 @@
       <c r="D15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>87</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>91</v>
@@ -1956,10 +2304,11 @@
         <v>22</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>92</v>
       </c>
@@ -1970,11 +2319,10 @@
         <v>22</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>94</v>
       </c>
@@ -1988,7 +2336,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>96</v>
       </c>
@@ -2002,7 +2350,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>98</v>
       </c>
@@ -2016,7 +2364,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -2030,7 +2378,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>102</v>
       </c>
@@ -2044,7 +2392,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -2058,7 +2406,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -2068,11 +2416,14 @@
       <c r="D25" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>108</v>
       </c>
@@ -2086,10 +2437,10 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>110</v>
       </c>
@@ -2106,7 +2457,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>112</v>
       </c>
@@ -2123,7 +2474,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -2137,10 +2488,10 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>116</v>
       </c>
@@ -2154,15 +2505,15 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>118</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>22</v>
@@ -2171,12 +2522,12 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>122</v>
@@ -2188,10 +2539,10 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>123</v>
       </c>
@@ -2208,7 +2559,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>125</v>
       </c>
@@ -2225,7 +2576,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>127</v>
       </c>
@@ -2242,7 +2593,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>129</v>
       </c>
@@ -2259,7 +2610,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>131</v>
       </c>
@@ -2276,7 +2627,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>133</v>
       </c>
@@ -2293,12 +2644,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>225</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>22</v>
@@ -2310,9 +2661,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>229</v>
+        <v>136</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>137</v>
@@ -2327,12 +2678,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>224</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>22</v>
@@ -2344,12 +2695,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>228</v>
+        <v>379</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>140</v>
+        <v>380</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>22</v>
@@ -2361,12 +2712,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>22</v>
@@ -2378,12 +2729,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>22</v>
@@ -2395,12 +2746,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>22</v>
@@ -2412,12 +2763,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>22</v>
@@ -2429,12 +2780,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>22</v>
@@ -2446,12 +2797,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>22</v>
@@ -2463,12 +2814,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>22</v>
@@ -2480,12 +2831,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>22</v>
@@ -2497,12 +2848,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>157</v>
+        <v>235</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>22</v>
@@ -2511,15 +2862,15 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>239</v>
+        <v>157</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>22</v>
@@ -2528,15 +2879,15 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>161</v>
-      </c>
       <c r="B53" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>22</v>
@@ -2545,16 +2896,18 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>163</v>
+        <v>67</v>
+      </c>
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>164</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
         <v>22</v>
       </c>
@@ -2564,16 +2917,14 @@
       <c r="H54" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J54" s="1"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>165</v>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>163</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C55" s="1"/>
+        <v>164</v>
+      </c>
       <c r="D55" s="1" t="s">
         <v>22</v>
       </c>
@@ -2581,15 +2932,15 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>22</v>
@@ -2598,16 +2949,17 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>169</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>170</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
         <v>22</v>
       </c>
@@ -2615,17 +2967,18 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>171</v>
+        <v>88</v>
+      </c>
+      <c r="K57" s="1"/>
+      <c r="M57" s="1"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>169</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C58" s="1"/>
+        <v>170</v>
+      </c>
       <c r="D58" s="1" t="s">
         <v>22</v>
       </c>
@@ -2633,18 +2986,18 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K58" s="1"/>
-      <c r="M58" s="1"/>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>173</v>
+        <v>67</v>
+      </c>
+      <c r="L58" s="1"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>174</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
         <v>22</v>
       </c>
@@ -2654,14 +3007,14 @@
       <c r="H59" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="L59" s="1"/>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M59" s="1"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
@@ -2673,14 +3026,13 @@
       <c r="H60" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M60" s="1"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
@@ -2693,12 +3045,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
@@ -2708,15 +3060,16 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>182</v>
+        <v>155</v>
+      </c>
+      <c r="M62" s="1"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>179</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
@@ -2726,16 +3079,16 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="M63" s="1"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>183</v>
+        <v>67</v>
+      </c>
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
@@ -2747,14 +3100,14 @@
       <c r="H64" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J64" s="1"/>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M64" s="1"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1" t="s">
@@ -2766,14 +3119,13 @@
       <c r="H65" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M65" s="1"/>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1" t="s">
@@ -2785,13 +3137,14 @@
       <c r="H66" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L66" s="1"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
@@ -2801,16 +3154,16 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L67" s="1"/>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="M67" s="1"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
@@ -2820,16 +3173,16 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="M68" s="1"/>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="L68" s="1"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
@@ -2839,16 +3192,15 @@
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L69" s="1"/>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>196</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>193</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
@@ -2858,15 +3210,16 @@
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="L70" s="1"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>197</v>
+        <v>236</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
@@ -2876,16 +3229,15 @@
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="L71" s="1"/>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>240</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
@@ -2895,15 +3247,16 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>200</v>
+        <v>67</v>
+      </c>
+      <c r="L72" s="1"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>198</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
@@ -2913,16 +3266,15 @@
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L73" s="1"/>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>202</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
@@ -2932,15 +3284,15 @@
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>205</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>202</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
@@ -2950,15 +3302,17 @@
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>206</v>
+        <v>155</v>
+      </c>
+      <c r="J75" s="1"/>
+      <c r="N75" s="1"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
+        <v>204</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
@@ -2968,17 +3322,15 @@
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="J76" s="1"/>
-      <c r="N76" s="1"/>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>208</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>206</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1" t="s">
@@ -2990,13 +3342,14 @@
       <c r="H77" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>210</v>
+      <c r="L77" s="1"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
@@ -3008,14 +3361,13 @@
       <c r="H78" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="L78" s="1"/>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
@@ -3028,12 +3380,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
@@ -3046,12 +3398,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
@@ -3064,12 +3416,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
@@ -3079,15 +3431,16 @@
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>220</v>
+        <v>155</v>
+      </c>
+      <c r="M82" s="1"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>218</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
@@ -3097,16 +3450,15 @@
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="M83" s="1"/>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
@@ -3116,15 +3468,16 @@
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="L84" s="1"/>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1" t="s">
@@ -3134,50 +3487,50 @@
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1" t="s">
-        <v>67</v>
+        <v>241</v>
       </c>
       <c r="L85" s="1"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
       <c r="H86" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="L86" s="1"/>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
       <c r="H87" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="L87" s="1"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1" t="s">
@@ -3189,14 +3542,13 @@
       <c r="H88" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="L88" s="1"/>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
@@ -3206,15 +3558,15 @@
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
@@ -3224,15 +3576,15 @@
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
       <c r="H90" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>238</v>
+        <v>386</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
@@ -3242,15 +3594,17 @@
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
       <c r="H91" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="J91" s="1"/>
+      <c r="L91" s="1"/>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1" t="s">
@@ -3260,17 +3614,15 @@
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="J92" s="1"/>
-      <c r="L92" s="1"/>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>242</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1" t="s">
@@ -3280,15 +3632,16 @@
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
       <c r="H93" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>247</v>
+        <v>67</v>
+      </c>
+      <c r="K93" s="1"/>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
+        <v>244</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
@@ -3300,14 +3653,13 @@
       <c r="H94" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K94" s="1"/>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1" t="s">
@@ -3320,12 +3672,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1" t="s">
@@ -3335,15 +3687,15 @@
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="1" t="s">
@@ -3353,15 +3705,17 @@
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+      <c r="L97" s="1"/>
+      <c r="N97" s="1"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C98" s="1"/>
       <c r="D98" s="1" t="s">
@@ -3370,16 +3724,17 @@
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
-      <c r="H98" s="1"/>
+      <c r="H98" s="1" t="s">
+        <v>381</v>
+      </c>
       <c r="L98" s="1"/>
-      <c r="N98" s="1"/>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C99" s="1"/>
       <c r="D99" s="1" t="s">
@@ -3388,15 +3743,17 @@
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
-      <c r="H99" s="1"/>
+      <c r="H99" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="L99" s="1"/>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
@@ -3406,16 +3763,16 @@
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
       <c r="H100" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="L100" s="1"/>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="K100" s="1"/>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="1" t="s">
@@ -3425,15 +3782,15 @@
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
@@ -3443,15 +3800,17 @@
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
       <c r="H102" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="K102" s="1"/>
+      <c r="L102" s="1"/>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
@@ -3463,15 +3822,13 @@
       <c r="H103" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K103" s="1"/>
-      <c r="L103" s="1"/>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
@@ -3483,13 +3840,14 @@
       <c r="H104" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J104" s="1"/>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
@@ -3499,16 +3857,17 @@
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
       <c r="H105" s="1" t="s">
-        <v>67</v>
+        <v>155</v>
       </c>
       <c r="J105" s="1"/>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L105" s="1"/>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
@@ -3518,17 +3877,15 @@
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
       <c r="H106" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="J106" s="1"/>
-      <c r="L106" s="1"/>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
@@ -3538,15 +3895,15 @@
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
       <c r="H107" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>277</v>
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="1" t="s">
@@ -3556,15 +3913,15 @@
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
       <c r="H108" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1" t="s">
@@ -3573,14 +3930,16 @@
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
-      <c r="H109" s="1"/>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H109" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="1" t="s">
@@ -3593,12 +3952,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C111" s="1"/>
       <c r="D111" s="1" t="s">
@@ -3610,13 +3969,14 @@
       <c r="H111" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>283</v>
+      <c r="L111" s="1"/>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>280</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="1" t="s">
@@ -3626,16 +3986,15 @@
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L112" s="1"/>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>285</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A113" s="1" t="s">
+        <v>282</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="1" t="s">
@@ -3645,63 +4004,64 @@
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>287</v>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>284</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C114" s="1"/>
       <c r="D114" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E114" s="1"/>
-      <c r="F114" s="1"/>
-      <c r="G114" s="1"/>
       <c r="H114" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C115" s="1"/>
       <c r="D115" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>292</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A116" s="1" t="s">
+        <v>288</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C116" s="1"/>
       <c r="D116" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+      <c r="G116" s="1"/>
       <c r="H116" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="K116" s="1"/>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C117" s="1"/>
       <c r="D117" s="1" t="s">
@@ -3711,16 +4071,16 @@
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="K117" s="1"/>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="L117" s="1"/>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
@@ -3732,14 +4092,15 @@
       <c r="H118" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="K118" s="1"/>
       <c r="L118" s="1"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>298</v>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>294</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C119" s="1"/>
       <c r="D119" s="1" t="s">
@@ -3749,17 +4110,15 @@
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
       <c r="H119" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K119" s="1"/>
-      <c r="L119" s="1"/>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>299</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A120" s="1" t="s">
+        <v>296</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C120" s="1"/>
       <c r="D120" s="1" t="s">
@@ -3769,15 +4128,16 @@
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
       <c r="H120" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="K120" s="1"/>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C121" s="1"/>
       <c r="D121" s="1" t="s">
@@ -3791,12 +4151,12 @@
       </c>
       <c r="K121" s="1"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>303</v>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>300</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C122" s="1"/>
       <c r="D122" s="1" t="s">
@@ -3808,14 +4168,13 @@
       <c r="H122" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K122" s="1"/>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>305</v>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A123" s="1" t="s">
+        <v>302</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C123" s="1"/>
       <c r="D123" s="1" t="s">
@@ -3828,12 +4187,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C124" s="1"/>
       <c r="D124" s="1" t="s">
@@ -3846,12 +4205,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C125" s="1"/>
       <c r="D125" s="1" t="s">
@@ -3864,12 +4223,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C126" s="1"/>
       <c r="D126" s="1" t="s">
@@ -3882,12 +4241,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C127" s="1"/>
       <c r="D127" s="1" t="s">
@@ -3900,12 +4259,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B128" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>316</v>
       </c>
       <c r="C128" s="1"/>
       <c r="D128" s="1" t="s">
@@ -3918,12 +4277,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C129" s="1"/>
       <c r="D129" s="1" t="s">
@@ -3936,12 +4295,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C130" s="1"/>
       <c r="D130" s="1" t="s">
@@ -3951,15 +4310,15 @@
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
       <c r="H130" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C131" s="1"/>
       <c r="D131" s="1" t="s">
@@ -3969,15 +4328,15 @@
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
       <c r="H131" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
-        <v>324</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>321</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C132" s="1"/>
       <c r="D132" s="1" t="s">
@@ -3987,15 +4346,15 @@
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
       <c r="H132" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>326</v>
+        <v>381</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A133" s="1" t="s">
+        <v>323</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C133" s="1"/>
       <c r="D133" s="1" t="s">
@@ -4004,14 +4363,16 @@
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
-      <c r="H133" s="1"/>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H133" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C134" s="1"/>
       <c r="D134" s="1" t="s">
@@ -4020,16 +4381,14 @@
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
-      <c r="H134" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
-        <v>330</v>
+      <c r="H134" s="1"/>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>327</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C135" s="1"/>
       <c r="D135" s="1" t="s">
@@ -4038,14 +4397,16 @@
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
-      <c r="H135" s="1"/>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>332</v>
+      <c r="H135" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A136" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C136" s="1"/>
       <c r="D136" s="1" t="s">
@@ -4058,12 +4419,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C137" s="1"/>
       <c r="D137" s="1" t="s">
@@ -4075,13 +4436,14 @@
       <c r="H137" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M137" s="1"/>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C138" s="1"/>
       <c r="D138" s="1" t="s">
@@ -4093,14 +4455,13 @@
       <c r="H138" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M138" s="1"/>
-    </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="1" t="s">
@@ -4113,12 +4474,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C140" s="1"/>
       <c r="D140" s="1" t="s">
@@ -4128,15 +4489,16 @@
       <c r="F140" s="1"/>
       <c r="G140" s="1"/>
       <c r="H140" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="J140" s="1"/>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="1" t="s">
@@ -4146,16 +4508,15 @@
       <c r="F141" s="1"/>
       <c r="G141" s="1"/>
       <c r="H141" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="J141" s="1"/>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="1" t="s">
@@ -4168,12 +4529,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C143" s="1"/>
       <c r="D143" s="1" t="s">
@@ -4186,12 +4547,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C144" s="1"/>
       <c r="D144" s="1" t="s">
@@ -4204,12 +4565,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C145" s="1"/>
       <c r="D145" s="1" t="s">
@@ -4222,12 +4583,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C146" s="1"/>
       <c r="D146" s="1" t="s">
@@ -4240,12 +4601,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C147" s="1"/>
       <c r="D147" s="1" t="s">
@@ -4255,15 +4616,15 @@
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
       <c r="H147" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C148" s="1"/>
       <c r="D148" s="1" t="s">
@@ -4273,15 +4634,15 @@
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
       <c r="H148" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C149" s="1"/>
       <c r="D149" s="1" t="s">
@@ -4291,15 +4652,15 @@
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
       <c r="H149" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C150" s="1"/>
       <c r="D150" s="1" t="s">
@@ -4309,15 +4670,15 @@
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
       <c r="H150" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B151" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>363</v>
       </c>
       <c r="C151" s="1"/>
       <c r="D151" s="1" t="s">
@@ -4330,54 +4691,443 @@
         <v>67</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H152" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A153" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="B152" s="1" t="s">
+      <c r="C153" s="1"/>
+      <c r="D153" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E153" s="1"/>
+      <c r="F153" s="1"/>
+      <c r="G153" s="1"/>
+      <c r="H153" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A154" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C152" s="1"/>
-      <c r="D152" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E152" s="1"/>
-      <c r="F152" s="1"/>
-      <c r="G152" s="1"/>
-      <c r="H152" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="1" t="s">
+      <c r="B154" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C154" s="1"/>
+      <c r="D154" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E154" s="1"/>
+      <c r="F154" s="1"/>
+      <c r="G154" s="1"/>
+      <c r="H154" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A155" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B155" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B153" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H153" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H156" s="1"/>
+      <c r="C155" s="1"/>
+      <c r="D155" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E155" s="1"/>
+      <c r="F155" s="1"/>
+      <c r="G155" s="1"/>
+      <c r="H155" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A156" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C156" s="1"/>
+      <c r="D156" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E156" s="1"/>
+      <c r="F156" s="1"/>
+      <c r="G156" s="1"/>
+      <c r="H156" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A157" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C157" s="1"/>
+      <c r="D157" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E157" s="1"/>
+      <c r="F157" s="1"/>
+      <c r="G157" s="1"/>
+      <c r="H157" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A158" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C158" s="1"/>
+      <c r="D158" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E158" s="1"/>
+      <c r="F158" s="1"/>
+      <c r="G158" s="1"/>
+      <c r="H158" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A159" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C159" s="1"/>
+      <c r="D159" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E159" s="1"/>
+      <c r="F159" s="1"/>
+      <c r="G159" s="1"/>
+      <c r="H159" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A160" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C160" s="1"/>
+      <c r="D160" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E160" s="1"/>
+      <c r="F160" s="1"/>
+      <c r="G160" s="1"/>
+      <c r="H160" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A161" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C161" s="1"/>
+      <c r="D161" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E161" s="1"/>
+      <c r="F161" s="1"/>
+      <c r="G161" s="1"/>
+      <c r="H161" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A162" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C162" s="1"/>
+      <c r="D162" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E162" s="1"/>
+      <c r="F162" s="1"/>
+      <c r="G162" s="1"/>
+      <c r="H162" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A163" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C163" s="1"/>
+      <c r="D163" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E163" s="1"/>
+      <c r="F163" s="1"/>
+      <c r="G163" s="1"/>
+      <c r="H163" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A164" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C164" s="1"/>
+      <c r="D164" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E164" s="1"/>
+      <c r="F164" s="1"/>
+      <c r="G164" s="1"/>
+      <c r="H164" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A165" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C165" s="1"/>
+      <c r="D165" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E165" s="1"/>
+      <c r="F165" s="1"/>
+      <c r="G165" s="1"/>
+      <c r="H165" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A166" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C166" s="1"/>
+      <c r="D166" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E166" s="1"/>
+      <c r="F166" s="1"/>
+      <c r="G166" s="1"/>
+      <c r="H166" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A167" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C167" s="1"/>
+      <c r="D167" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E167" s="1"/>
+      <c r="F167" s="1"/>
+      <c r="G167" s="1"/>
+      <c r="H167" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A168" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C168" s="1"/>
+      <c r="D168" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E168" s="1"/>
+      <c r="F168" s="1"/>
+      <c r="G168" s="1"/>
+      <c r="H168" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A169" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C169" s="1"/>
+      <c r="D169" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E169" s="1"/>
+      <c r="F169" s="1"/>
+      <c r="G169" s="1"/>
+      <c r="H169" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A170" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C170" s="1"/>
+      <c r="D170" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E170" s="1"/>
+      <c r="F170" s="1"/>
+      <c r="G170" s="1"/>
+      <c r="H170" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A171" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C171" s="1"/>
+      <c r="D171" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E171" s="1"/>
+      <c r="F171" s="1"/>
+      <c r="G171" s="1"/>
+      <c r="H171" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A172" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="C172" s="1"/>
+      <c r="D172" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E172" s="1"/>
+      <c r="F172" s="1"/>
+      <c r="G172" s="1"/>
+      <c r="H172" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A173" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C173" s="1"/>
+      <c r="D173" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E173" s="1"/>
+      <c r="F173" s="1"/>
+      <c r="G173" s="1"/>
+      <c r="H173" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A174" s="1"/>
+      <c r="B174" s="1"/>
+      <c r="C174" s="1"/>
+      <c r="D174" s="1"/>
+      <c r="E174" s="1"/>
+      <c r="F174" s="1"/>
+      <c r="G174" s="1"/>
+      <c r="H174" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B1:B152 B154:B1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  <conditionalFormatting sqref="B175:B1048576 B1:B151">
+    <cfRule type="duplicateValues" dxfId="25" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A152 A154:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  <conditionalFormatting sqref="A175:A1048576 A1:A151">
+    <cfRule type="duplicateValues" dxfId="24" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B153">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="B152:B154">
+    <cfRule type="duplicateValues" dxfId="23" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A153">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="A152:A154">
+    <cfRule type="duplicateValues" dxfId="22" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B155">
+    <cfRule type="duplicateValues" dxfId="21" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A155">
+    <cfRule type="duplicateValues" dxfId="20" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B156">
+    <cfRule type="duplicateValues" dxfId="19" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A156">
+    <cfRule type="duplicateValues" dxfId="18" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B157:B174">
+    <cfRule type="duplicateValues" dxfId="0" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A157:A174">
+    <cfRule type="duplicateValues" dxfId="16" priority="16"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>